<commit_message>
Integration of OLS with Data
</commit_message>
<xml_diff>
--- a/Results/Summary Stats.xlsx
+++ b/Results/Summary Stats.xlsx
@@ -14,12 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>Employment</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>SGrowth_2023_2019</t>
+  </si>
+  <si>
+    <t>LSGrowth_2023_2019</t>
+  </si>
+  <si>
+    <t>Starting_INT</t>
+  </si>
+  <si>
+    <t>Starting_BS_Strength</t>
+  </si>
+  <si>
+    <t>Starting_Size_ln</t>
+  </si>
+  <si>
+    <t>Starting_Profit</t>
+  </si>
+  <si>
+    <t>HGX%</t>
   </si>
   <si>
     <t>count</t>
@@ -401,374 +416,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="C1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>1803</v>
+      </c>
+      <c r="C2">
+        <v>1803</v>
+      </c>
+      <c r="D2">
+        <v>1803</v>
+      </c>
+      <c r="E2">
+        <v>1803</v>
+      </c>
+      <c r="F2">
+        <v>1803</v>
+      </c>
+      <c r="G2">
+        <v>1803</v>
+      </c>
+      <c r="H2">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>48.94737648153436</v>
+      </c>
+      <c r="C3">
+        <v>0.2935806965605974</v>
+      </c>
+      <c r="D3">
+        <v>31.13338928682742</v>
+      </c>
+      <c r="E3">
+        <v>0.4200568445732775</v>
+      </c>
+      <c r="F3">
+        <v>13.47056692564208</v>
+      </c>
+      <c r="G3">
+        <v>0.03950992765804739</v>
+      </c>
+      <c r="H3">
+        <v>-0.009812136347166621</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>92.2230732451266</v>
+      </c>
+      <c r="C4">
+        <v>0.5413950655413687</v>
+      </c>
+      <c r="D4">
+        <v>35.17663190876191</v>
+      </c>
+      <c r="E4">
+        <v>0.2482900782140482</v>
+      </c>
+      <c r="F4">
+        <v>0.8453726038218823</v>
+      </c>
+      <c r="G4">
+        <v>0.07592963679441075</v>
+      </c>
+      <c r="H4">
+        <v>0.162304729528329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>-99.8852710128965</v>
+      </c>
+      <c r="C5">
+        <v>-6.770352751721602</v>
+      </c>
+      <c r="D5">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>1810</v>
-      </c>
-      <c r="D2">
-        <v>1810</v>
-      </c>
-      <c r="E2">
-        <v>1809</v>
-      </c>
-      <c r="F2">
-        <v>1810</v>
-      </c>
-      <c r="G2">
-        <v>1810</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>1242684.414967931</v>
-      </c>
-      <c r="D3">
-        <v>1244264.435434976</v>
-      </c>
-      <c r="E3">
-        <v>1490712.432084339</v>
-      </c>
-      <c r="F3">
-        <v>1881326.503547316</v>
-      </c>
-      <c r="G3">
-        <v>1943663.434254501</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>2646641.536156968</v>
-      </c>
-      <c r="D4">
-        <v>2804005.191364285</v>
-      </c>
-      <c r="E4">
-        <v>3305455.34824124</v>
-      </c>
-      <c r="F4">
-        <v>4351675.289896734</v>
-      </c>
-      <c r="G4">
-        <v>5119725.265028626</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>193371</v>
-      </c>
-      <c r="D5">
-        <v>76744</v>
-      </c>
       <c r="E5">
-        <v>7380</v>
+        <v>-1.43996073261185</v>
       </c>
       <c r="F5">
-        <v>12233</v>
+        <v>12.17236590246427</v>
       </c>
       <c r="G5">
-        <v>393.743</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>-0.6982980223725119</v>
+      </c>
+      <c r="H5">
+        <v>-0.9965545290052217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>14.52204435477605</v>
       </c>
       <c r="C6">
-        <v>378139.25</v>
+        <v>0.1355971422632631</v>
       </c>
       <c r="D6">
-        <v>374104.409235</v>
+        <v>0.1299400835988426</v>
       </c>
       <c r="E6">
-        <v>437350.97875</v>
+        <v>0.2529723413193963</v>
       </c>
       <c r="F6">
-        <v>520579.85423</v>
+        <v>12.8424259011645</v>
       </c>
       <c r="G6">
-        <v>512918.2833175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>0.008283067495853256</v>
+      </c>
+      <c r="H6">
+        <v>-0.01899421591852191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>38.17163419627651</v>
       </c>
       <c r="C7">
-        <v>556991.0738649999</v>
+        <v>0.3233264524425223</v>
       </c>
       <c r="D7">
-        <v>550340.5</v>
+        <v>14.03332244629682</v>
       </c>
       <c r="E7">
-        <v>673169</v>
+        <v>0.4115027799527248</v>
       </c>
       <c r="F7">
-        <v>826146</v>
+        <v>13.22765989101407</v>
       </c>
       <c r="G7">
-        <v>809442.67556</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>0.02606610460031464</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>65.61888515584661</v>
       </c>
       <c r="C8">
-        <v>1020723</v>
+        <v>0.504519090053293</v>
       </c>
       <c r="D8">
-        <v>1015698.17241</v>
+        <v>61.31606276349302</v>
       </c>
       <c r="E8">
-        <v>1195422</v>
+        <v>0.5918077795627114</v>
       </c>
       <c r="F8">
-        <v>1454891</v>
+        <v>13.82922602091509</v>
       </c>
       <c r="G8">
-        <v>1499395.3293225</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>0.05807013692235607</v>
+      </c>
+      <c r="H8">
+        <v>0.01991921880719105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>2732.350803043111</v>
       </c>
       <c r="C9">
-        <v>55573747.04</v>
+        <v>3.343692132285168</v>
       </c>
       <c r="D9">
-        <v>61216804.38</v>
+        <v>100.0001044521693</v>
       </c>
       <c r="E9">
-        <v>68246695.47</v>
+        <v>0.9832084167935834</v>
       </c>
       <c r="F9">
-        <v>85034775</v>
+        <v>17.83322147217127</v>
       </c>
       <c r="G9">
-        <v>98022928</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>1810</v>
-      </c>
-      <c r="D10">
-        <v>1805</v>
-      </c>
-      <c r="E10">
-        <v>1805</v>
-      </c>
-      <c r="F10">
-        <v>1808</v>
-      </c>
-      <c r="G10">
-        <v>1810</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>1601.458378913444</v>
-      </c>
-      <c r="D11">
-        <v>1431.557057248384</v>
-      </c>
-      <c r="E11">
-        <v>1454.79011634349</v>
-      </c>
-      <c r="F11">
-        <v>1454.802909292036</v>
-      </c>
-      <c r="G11">
-        <v>1501.154045546961</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>7222.403606315214</v>
-      </c>
-      <c r="D12">
-        <v>4046.66771236788</v>
-      </c>
-      <c r="E12">
-        <v>4067.283674780733</v>
-      </c>
-      <c r="F12">
-        <v>4049.684951842819</v>
-      </c>
-      <c r="G12">
-        <v>4399.958327456047</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14">
-        <v>232</v>
-      </c>
-      <c r="D14">
-        <v>228</v>
-      </c>
-      <c r="E14">
-        <v>234</v>
-      </c>
-      <c r="F14">
-        <v>238</v>
-      </c>
-      <c r="G14">
-        <v>241.25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15">
-        <v>520.5</v>
-      </c>
-      <c r="D15">
-        <v>513</v>
-      </c>
-      <c r="E15">
-        <v>527</v>
-      </c>
-      <c r="F15">
-        <v>531.5</v>
-      </c>
-      <c r="G15">
-        <v>531.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16">
-        <v>1208.75</v>
-      </c>
-      <c r="D16">
-        <v>1178</v>
-      </c>
-      <c r="E16">
-        <v>1192</v>
-      </c>
-      <c r="F16">
-        <v>1206.5</v>
-      </c>
-      <c r="G16">
-        <v>1202.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17">
-        <v>238033</v>
-      </c>
-      <c r="D17">
-        <v>78873</v>
-      </c>
-      <c r="E17">
-        <v>74350.5</v>
-      </c>
-      <c r="F17">
-        <v>77726.7</v>
-      </c>
-      <c r="G17">
-        <v>79292</v>
+        <v>0.9036493945910843</v>
+      </c>
+      <c r="H9">
+        <v>0.9967764644841388</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A17"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>